<commit_message>
Added some more functionality to show the remainder of the days of the week left after "Today" and "Tomorrow". Will also loop through all appointments and calculate if a slot is available
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\GoogleCalendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BBF0D27-B1AA-4D0F-AE9D-900BA5B7860E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28933C30-6B80-43E8-9362-5793AF2B13B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{564E1D42-0E07-4D1A-984B-FD5260481A8F}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{564E1D42-0E07-4D1A-984B-FD5260481A8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="8">
   <si>
     <t>Busy</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>Duration = 60min</t>
   </si>
   <si>
     <t>ok</t>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>30min</t>
+  </si>
+  <si>
+    <t>90Min</t>
   </si>
 </sst>
 </file>
@@ -406,47 +406,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71911044-805F-432F-95F2-F51881748D23}">
-  <dimension ref="B2:R18"/>
+  <dimension ref="B2:X53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L2" t="s">
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="S2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>5</v>
+      </c>
+      <c r="W2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>0.34375</v>
       </c>
@@ -478,10 +493,28 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="P3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="T3" t="s">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="X3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>0.35416666666666669</v>
       </c>
@@ -512,8 +545,26 @@
       <c r="O4" s="1">
         <v>0.34375</v>
       </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R4" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0.34375</v>
+      </c>
+      <c r="T4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="W4" s="1">
+        <v>0.34375</v>
+      </c>
+      <c r="X4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>0.36458333333333331</v>
       </c>
@@ -544,8 +595,26 @@
       <c r="O5" s="1">
         <v>0.35416666666666669</v>
       </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R5" s="1">
+        <v>0.40625</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="T5" t="s">
+        <v>2</v>
+      </c>
+      <c r="V5" s="1">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="W5" s="1">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="X5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>0.375</v>
       </c>
@@ -576,8 +645,26 @@
       <c r="O6" s="1">
         <v>0.36458333333333298</v>
       </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R6" s="1">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0.36458333333333298</v>
+      </c>
+      <c r="T6" t="s">
+        <v>2</v>
+      </c>
+      <c r="V6" s="1">
+        <v>0.39583333333333298</v>
+      </c>
+      <c r="W6" s="1">
+        <v>0.36458333333333298</v>
+      </c>
+      <c r="X6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>0.38541666666666702</v>
       </c>
@@ -608,8 +695,26 @@
       <c r="O7" s="1">
         <v>0.41666666666666702</v>
       </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R7" s="1">
+        <v>0.42708333333333298</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="T7" t="s">
+        <v>2</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0.40625</v>
+      </c>
+      <c r="W7" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="X7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>0.39583333333333298</v>
       </c>
@@ -640,8 +745,26 @@
       <c r="O8" s="1">
         <v>0.42708333333333298</v>
       </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R8" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0.38541666666666702</v>
+      </c>
+      <c r="T8" t="s">
+        <v>2</v>
+      </c>
+      <c r="V8" s="1">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="W8" s="1">
+        <v>0.38541666666666702</v>
+      </c>
+      <c r="X8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>0.40625</v>
       </c>
@@ -672,8 +795,26 @@
       <c r="O9" s="1">
         <v>0.4375</v>
       </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R9" s="1">
+        <v>0.44791666666666602</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0.39583333333333298</v>
+      </c>
+      <c r="T9" t="s">
+        <v>1</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0.42708333333333298</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0.39583333333333298</v>
+      </c>
+      <c r="X9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>0.41666666666666702</v>
       </c>
@@ -704,8 +845,26 @@
       <c r="O10" s="1">
         <v>0.44791666666666702</v>
       </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R10" s="1">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0.40625</v>
+      </c>
+      <c r="T10" t="s">
+        <v>1</v>
+      </c>
+      <c r="V10" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="W10" s="1">
+        <v>0.40625</v>
+      </c>
+      <c r="X10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>0.42708333333333298</v>
       </c>
@@ -736,8 +895,26 @@
       <c r="O11" s="1">
         <v>0.45833333333333298</v>
       </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R11" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="T11" t="s">
+        <v>1</v>
+      </c>
+      <c r="V11" s="1">
+        <v>0.44791666666666702</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="X11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>0.4375</v>
       </c>
@@ -768,8 +945,26 @@
       <c r="O12" s="1">
         <v>0.46875</v>
       </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R12" s="1">
+        <v>0.47916666666666602</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0.42708333333333298</v>
+      </c>
+      <c r="T12" t="s">
+        <v>1</v>
+      </c>
+      <c r="V12" s="1">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="W12" s="1">
+        <v>0.42708333333333298</v>
+      </c>
+      <c r="X12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>0.44791666666666702</v>
       </c>
@@ -800,8 +995,26 @@
       <c r="O13" s="1">
         <v>0.47916666666666702</v>
       </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R13" s="1">
+        <v>0.48958333333333298</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="T13" t="s">
+        <v>1</v>
+      </c>
+      <c r="V13" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="W13" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="X13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>0.45833333333333398</v>
       </c>
@@ -832,8 +1045,26 @@
       <c r="O14" s="1">
         <v>0.48958333333333298</v>
       </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="S14" s="1">
+        <v>0.44791666666666702</v>
+      </c>
+      <c r="T14" t="s">
+        <v>1</v>
+      </c>
+      <c r="V14" s="1">
+        <v>0.47916666666666702</v>
+      </c>
+      <c r="W14" s="1">
+        <v>0.44791666666666702</v>
+      </c>
+      <c r="X14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>0.46875</v>
       </c>
@@ -861,8 +1092,26 @@
       <c r="L15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R15" s="1">
+        <v>0.51041666666666696</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="T15" t="s">
+        <v>1</v>
+      </c>
+      <c r="V15" s="1">
+        <v>0.48958333333333298</v>
+      </c>
+      <c r="W15" s="1">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="X15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>0.47916666666666702</v>
       </c>
@@ -888,10 +1137,28 @@
         <v>0.46875</v>
       </c>
       <c r="L16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0.52083333333333304</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="T16" t="s">
+        <v>1</v>
+      </c>
+      <c r="V16" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="W16" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="X16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>0.48958333333333398</v>
       </c>
@@ -917,10 +1184,28 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="L17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0.53125</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0.47916666666666702</v>
+      </c>
+      <c r="T17" t="s">
+        <v>1</v>
+      </c>
+      <c r="V17" s="1">
+        <v>0.51041666666666696</v>
+      </c>
+      <c r="W17" s="1">
+        <v>0.47916666666666702</v>
+      </c>
+      <c r="X17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>0.5</v>
       </c>
@@ -948,6 +1233,666 @@
       <c r="L18" t="s">
         <v>1</v>
       </c>
+      <c r="R18" s="1">
+        <v>0.54166666666666596</v>
+      </c>
+      <c r="S18" s="1">
+        <v>0.48958333333333298</v>
+      </c>
+      <c r="T18" t="s">
+        <v>1</v>
+      </c>
+      <c r="V18" s="1">
+        <v>0.52083333333333304</v>
+      </c>
+      <c r="W18" s="1">
+        <v>0.48958333333333298</v>
+      </c>
+      <c r="X18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="J19" s="1">
+        <v>0.53125</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L19" t="s">
+        <v>1</v>
+      </c>
+      <c r="V19" s="1">
+        <v>0.53125</v>
+      </c>
+      <c r="W19" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="X19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="J20" s="1">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.51041666666666696</v>
+      </c>
+      <c r="L20" t="s">
+        <v>1</v>
+      </c>
+      <c r="V20" s="1">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="W20" s="1">
+        <v>0.51041666666666696</v>
+      </c>
+      <c r="X20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="J21" s="1">
+        <v>0.55208333333333304</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0.52083333333333304</v>
+      </c>
+      <c r="L21" t="s">
+        <v>1</v>
+      </c>
+      <c r="V21" s="1">
+        <v>0.55208333333333304</v>
+      </c>
+      <c r="W21" s="1">
+        <v>0.52083333333333304</v>
+      </c>
+      <c r="X21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="J22" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.53125</v>
+      </c>
+      <c r="L22" t="s">
+        <v>1</v>
+      </c>
+      <c r="V22" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="W22" s="1">
+        <v>0.53125</v>
+      </c>
+      <c r="X22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="J23" s="1">
+        <v>0.57291666666666696</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="L23" t="s">
+        <v>2</v>
+      </c>
+      <c r="V23" s="1">
+        <v>0.57291666666666696</v>
+      </c>
+      <c r="W23" s="1">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="X23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="J24" s="1">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0.55208333333333304</v>
+      </c>
+      <c r="L24" t="s">
+        <v>2</v>
+      </c>
+      <c r="V24" s="1">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="W24" s="1">
+        <v>0.55208333333333304</v>
+      </c>
+      <c r="X24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="J25" s="1">
+        <v>0.59375</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="L25" t="s">
+        <v>2</v>
+      </c>
+      <c r="V25" s="1">
+        <v>0.59375</v>
+      </c>
+      <c r="W25" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="X25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="J26" s="1">
+        <v>0.60416666666666696</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0.57291666666666696</v>
+      </c>
+      <c r="L26" t="s">
+        <v>2</v>
+      </c>
+      <c r="V26" s="1">
+        <v>0.60416666666666696</v>
+      </c>
+      <c r="W26" s="1">
+        <v>0.57291666666666696</v>
+      </c>
+      <c r="X26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="J27" s="1">
+        <v>0.61458333333333304</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="L27" t="s">
+        <v>2</v>
+      </c>
+      <c r="V27" s="1">
+        <v>0.61458333333333304</v>
+      </c>
+      <c r="W27" s="1">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="X27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="J28" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0.59375</v>
+      </c>
+      <c r="L28" t="s">
+        <v>2</v>
+      </c>
+      <c r="V28" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="W28" s="1">
+        <v>0.59375</v>
+      </c>
+      <c r="X28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="J29" s="1">
+        <v>0.63541666666666696</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0.60416666666666696</v>
+      </c>
+      <c r="L29" t="s">
+        <v>2</v>
+      </c>
+      <c r="V29" s="1">
+        <v>0.63541666666666696</v>
+      </c>
+      <c r="W29" s="1">
+        <v>0.60416666666666696</v>
+      </c>
+      <c r="X29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="J30" s="1">
+        <v>0.64583333333333304</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0.61458333333333304</v>
+      </c>
+      <c r="L30" t="s">
+        <v>2</v>
+      </c>
+      <c r="V30" s="1">
+        <v>0.64583333333333304</v>
+      </c>
+      <c r="W30" s="1">
+        <v>0.61458333333333304</v>
+      </c>
+      <c r="X30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="J31" s="1">
+        <v>0.65625</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="L31" t="s">
+        <v>2</v>
+      </c>
+      <c r="V31" s="1">
+        <v>0.65625</v>
+      </c>
+      <c r="W31" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="X31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="J32" s="1">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0.63541666666666696</v>
+      </c>
+      <c r="L32" t="s">
+        <v>2</v>
+      </c>
+      <c r="V32" s="1">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="W32" s="1">
+        <v>0.63541666666666696</v>
+      </c>
+      <c r="X32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J33" s="1">
+        <v>0.67708333333333404</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0.64583333333333404</v>
+      </c>
+      <c r="L33" t="s">
+        <v>2</v>
+      </c>
+      <c r="V33" s="1">
+        <v>0.67708333333333404</v>
+      </c>
+      <c r="W33" s="1">
+        <v>0.64583333333333404</v>
+      </c>
+      <c r="X33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J34" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0.65625</v>
+      </c>
+      <c r="L34" t="s">
+        <v>2</v>
+      </c>
+      <c r="V34" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="W34" s="1">
+        <v>0.65625</v>
+      </c>
+      <c r="X34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J35" s="1">
+        <v>0.69791666666666696</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="L35" t="s">
+        <v>2</v>
+      </c>
+      <c r="V35" s="1">
+        <v>0.69791666666666696</v>
+      </c>
+      <c r="W35" s="1">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="X35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J36" s="1">
+        <v>0.70833333333333703</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0.67708333333333404</v>
+      </c>
+      <c r="L36" t="s">
+        <v>2</v>
+      </c>
+      <c r="V36" s="1">
+        <v>0.70833333333333703</v>
+      </c>
+      <c r="W36" s="1">
+        <v>0.67708333333333404</v>
+      </c>
+      <c r="X36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J37" s="1">
+        <v>0.718750000000004</v>
+      </c>
+      <c r="K37" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="L37" t="s">
+        <v>1</v>
+      </c>
+      <c r="V37" s="1">
+        <v>0.718750000000004</v>
+      </c>
+      <c r="W37" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="X37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J38" s="1">
+        <v>0.72916666666666996</v>
+      </c>
+      <c r="K38" s="1">
+        <v>0.69791666666666696</v>
+      </c>
+      <c r="L38" t="s">
+        <v>1</v>
+      </c>
+      <c r="V38" s="1">
+        <v>0.72916666666666996</v>
+      </c>
+      <c r="W38" s="1">
+        <v>0.69791666666666696</v>
+      </c>
+      <c r="X38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J39" s="1">
+        <v>0.73958333333333703</v>
+      </c>
+      <c r="K39" s="1">
+        <v>0.70833333333333404</v>
+      </c>
+      <c r="L39" t="s">
+        <v>1</v>
+      </c>
+      <c r="V39" s="1">
+        <v>0.73958333333333703</v>
+      </c>
+      <c r="W39" s="1">
+        <v>0.70833333333333404</v>
+      </c>
+      <c r="X39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J40" s="1">
+        <v>0.750000000000004</v>
+      </c>
+      <c r="K40" s="1">
+        <v>0.71875</v>
+      </c>
+      <c r="L40" t="s">
+        <v>1</v>
+      </c>
+      <c r="V40" s="1">
+        <v>0.750000000000004</v>
+      </c>
+      <c r="W40" s="1">
+        <v>0.71875</v>
+      </c>
+      <c r="X40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J41" s="1">
+        <v>0.76041666666667096</v>
+      </c>
+      <c r="K41" s="1">
+        <v>0.72916666666666696</v>
+      </c>
+      <c r="L41" t="s">
+        <v>1</v>
+      </c>
+      <c r="V41" s="1">
+        <v>0.76041666666667096</v>
+      </c>
+      <c r="W41" s="1">
+        <v>0.72916666666666696</v>
+      </c>
+      <c r="X41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J42" s="1">
+        <v>0.77083333333333803</v>
+      </c>
+      <c r="K42" s="1">
+        <v>0.73958333333333404</v>
+      </c>
+      <c r="L42" t="s">
+        <v>1</v>
+      </c>
+      <c r="V42" s="1">
+        <v>0.77083333333333803</v>
+      </c>
+      <c r="W42" s="1">
+        <v>0.73958333333333404</v>
+      </c>
+      <c r="X42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J43" s="1">
+        <v>0.781250000000005</v>
+      </c>
+      <c r="K43" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="L43" t="s">
+        <v>1</v>
+      </c>
+      <c r="V43" s="1">
+        <v>0.781250000000005</v>
+      </c>
+      <c r="W43" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="X43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J44" s="1">
+        <v>0.79166666666667296</v>
+      </c>
+      <c r="K44" s="1">
+        <v>0.76041666666666896</v>
+      </c>
+      <c r="V44" s="1">
+        <v>0.79166666666667296</v>
+      </c>
+      <c r="W44" s="1">
+        <v>0.76041666666666896</v>
+      </c>
+      <c r="X44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J45" s="1">
+        <v>0.80208333333334003</v>
+      </c>
+      <c r="K45" s="1">
+        <v>0.77083333333333603</v>
+      </c>
+      <c r="V45" s="1">
+        <v>0.80208333333334003</v>
+      </c>
+      <c r="W45" s="1">
+        <v>0.77083333333333603</v>
+      </c>
+      <c r="X45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J46" s="1">
+        <v>0.81250000000000699</v>
+      </c>
+      <c r="K46" s="1">
+        <v>0.781250000000004</v>
+      </c>
+      <c r="V46" s="1">
+        <v>0.81250000000000699</v>
+      </c>
+      <c r="W46" s="1">
+        <v>0.781250000000004</v>
+      </c>
+      <c r="X46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J47" s="1">
+        <v>0.82291666666667396</v>
+      </c>
+      <c r="K47" s="1">
+        <v>0.79166666666667096</v>
+      </c>
+      <c r="V47" s="1">
+        <v>0.82291666666667396</v>
+      </c>
+      <c r="W47" s="1">
+        <v>0.79166666666667096</v>
+      </c>
+      <c r="X47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J48" s="1">
+        <v>0.83333333333334103</v>
+      </c>
+      <c r="K48" s="1">
+        <v>0.80208333333333803</v>
+      </c>
+      <c r="V48" s="1">
+        <v>0.83333333333334103</v>
+      </c>
+      <c r="W48" s="1">
+        <v>0.80208333333333803</v>
+      </c>
+      <c r="X48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J49" s="1">
+        <v>0.84375000000000799</v>
+      </c>
+      <c r="K49" s="1">
+        <v>0.812500000000005</v>
+      </c>
+      <c r="V49" s="1">
+        <v>0.84375000000000799</v>
+      </c>
+      <c r="W49" s="1">
+        <v>0.812500000000005</v>
+      </c>
+      <c r="X49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J50" s="1">
+        <v>0.85416666666667396</v>
+      </c>
+      <c r="K50" s="1">
+        <v>0.82291666666667196</v>
+      </c>
+      <c r="V50" s="1">
+        <v>0.85416666666667396</v>
+      </c>
+      <c r="W50" s="1">
+        <v>0.82291666666667196</v>
+      </c>
+      <c r="X50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J51" s="1">
+        <v>0.86458333333334103</v>
+      </c>
+      <c r="K51" s="1">
+        <v>0.83333333333333903</v>
+      </c>
+      <c r="V51" s="1">
+        <v>0.86458333333334103</v>
+      </c>
+      <c r="W51" s="1">
+        <v>0.83333333333333903</v>
+      </c>
+      <c r="X51" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="10:24" x14ac:dyDescent="0.25">
+      <c r="J53" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>